<commit_message>
Update kintis metrics spreadsheet with all functions' static analysis
</commit_message>
<xml_diff>
--- a/static-metrics/code-metrics-data/metrics-of-kintis-methods.xlsx
+++ b/static-metrics/code-metrics-data/metrics-of-kintis-methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steng\Desktop\mutation-analysis\mutation-research-jupyter-wk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steng\Desktop\mutation-analysis\kintis-funcs-updated\static-metrics\code-metrics-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D0B95-829F-469B-9D37-706385C0E66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5844206A-83E6-49AA-A43E-54DCB674D95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>